<commit_message>
Skapat while-loop och adderat funktioner
Programmet är färdigt för nu.
Eventuellt ska jag använda de två filerna som är över nu för att addera
prognoser till KPIF och arbetslöshet då det finns mycket data att ta av
där och kan kanske vara lite mer förutsägbara än bostadspriser hehe.
</commit_message>
<xml_diff>
--- a/kpif-stats-medianyear.xlsx
+++ b/kpif-stats-medianyear.xlsx
@@ -1,37 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus Turesson\Desktop\PythonProject4School\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2649C358-5257-4266-A05D-D5ACD10DBB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>KPIF</t>
+  </si>
+  <si>
+    <t>År</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +63,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,316 +387,308 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Datum</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>KPIF</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1988</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>5.55</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1989</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>6.3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>1990</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>10.1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>1991</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>9.5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>1992</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>1.75</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>1993</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>5.05</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>1994</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>2.4</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>1995</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>2.65</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>1996</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>1.3</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>1997</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1.7</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>1998</v>
       </c>
-      <c r="B12" t="n">
-        <v>1.15</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+      <c r="B12">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>1999</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1.3</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>2000</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>2001</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>2.7</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>2002</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>2.1</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>2003</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>2.4</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>2004</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>1.2</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>2005</v>
       </c>
-      <c r="B19" t="n">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+      <c r="B19">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>2006</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>1.35</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>2007</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>1.35</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>2008</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>2.7</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>2009</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>1.65</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>2010</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>1.9</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>2011</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>1.5</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>2012</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>0.9</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>2013</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>0.9</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>2014</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>0.5</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>2015</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>0.9</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>2016</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>1.4</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>2017</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>1.95</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>2018</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>2.15</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>2019</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>1.7</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>2020</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>0.5</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>2021</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>2.25</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>2022</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>8.25</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>2023</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>6.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixade lite efter redovisningen
Försökte mig på att skapa en prognos för framtiden men skrotade det
tillslut då det inte fanns ett enkelt linjärt samband i datan för att
kunna göra det snabbt. Jag nöjer mig här och låter datan vara :)
</commit_message>
<xml_diff>
--- a/kpif-stats-medianyear.xlsx
+++ b/kpif-stats-medianyear.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus Turesson\Desktop\PythonProject4School\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2649C358-5257-4266-A05D-D5ACD10DBB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8806FD25-91FB-40FA-A5C2-53281A41EDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,9 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>